<commit_message>
fixed table DCI export bug
</commit_message>
<xml_diff>
--- a/doc/misc/database_sizing.xlsx
+++ b/doc/misc/database_sizing.xlsx
@@ -5,250 +5,255 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="One Table per Node" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="78">
   <si>
-    <t>Minimum Row size with varchar</t>
-  </si>
-  <si>
-    <t>Average Row size with varchar</t>
-  </si>
-  <si>
-    <t>Row size with int</t>
-  </si>
-  <si>
-    <t>qty</t>
-  </si>
-  <si>
-    <t>size</t>
-  </si>
-  <si>
-    <t>total</t>
-  </si>
-  <si>
-    <t>2.f</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>2.v</t>
-  </si>
-  <si>
-    <t>varchars</t>
-  </si>
-  <si>
-    <t>2.s</t>
-  </si>
-  <si>
-    <t>varchar Max total</t>
-  </si>
-  <si>
-    <t>null bitmap</t>
-  </si>
-  <si>
-    <t>4.e</t>
-  </si>
-  <si>
-    <t>varchar estimated size</t>
-  </si>
-  <si>
-    <t>4.s</t>
-  </si>
-  <si>
-    <t>varchar size</t>
-  </si>
-  <si>
-    <t>Data Row Size</t>
-  </si>
-  <si>
-    <t>Bytes</t>
-  </si>
-  <si>
-    <t>dci's</t>
-  </si>
-  <si>
-    <t>nodes</t>
-  </si>
-  <si>
-    <t>polling</t>
-  </si>
-  <si>
-    <t>seconds</t>
-  </si>
-  <si>
-    <t>retention</t>
-  </si>
-  <si>
-    <t>days</t>
-  </si>
-  <si>
-    <t># of records per DCI</t>
-  </si>
-  <si>
-    <t># of records per node (# of rows)</t>
-  </si>
-  <si>
-    <t># of records total</t>
-  </si>
-  <si>
-    <t>Size of SQL data</t>
-  </si>
-  <si>
-    <t>Numer of rows per page</t>
-  </si>
-  <si>
-    <t>Clustered Index - 90% fill</t>
-  </si>
-  <si>
-    <t>Pages</t>
-  </si>
-  <si>
-    <t>Table Size (Data_Space_Used)</t>
-  </si>
-  <si>
-    <t>KB</t>
-  </si>
-  <si>
-    <t>MB</t>
-  </si>
-  <si>
-    <t>GB</t>
-  </si>
-  <si>
-    <t>Clustered Index Details</t>
-  </si>
-  <si>
-    <t>1.c</t>
-  </si>
-  <si>
-    <t>Number of Columns in Index</t>
-  </si>
-  <si>
-    <t>1.f</t>
-  </si>
-  <si>
-    <t>Number of Bytes of int cols in index</t>
-  </si>
-  <si>
-    <t>1.v</t>
-  </si>
-  <si>
-    <t>Number of varchar in index</t>
-  </si>
-  <si>
-    <t>1.s</t>
-  </si>
-  <si>
-    <t>Max Size of varchar in index</t>
-  </si>
-  <si>
-    <t>null bitmap in index</t>
-  </si>
-  <si>
-    <t>varchar index size</t>
-  </si>
-  <si>
-    <t>Index Row Size</t>
-  </si>
-  <si>
-    <t>Size of the Clustered Index</t>
-  </si>
-  <si>
-    <t>Index Rows Per page</t>
-  </si>
-  <si>
-    <t>6.0</t>
-  </si>
-  <si>
-    <t>Pages Level 0</t>
-  </si>
-  <si>
-    <t>Pages Level 1</t>
-  </si>
-  <si>
-    <t>Pages Level 2</t>
-  </si>
-  <si>
-    <t>6.n</t>
-  </si>
-  <si>
-    <t>{Note:  Repeat untl Pages Level n = 1}</t>
-  </si>
-  <si>
-    <t>6.t</t>
-  </si>
-  <si>
-    <t>Total Number of Pages</t>
-  </si>
-  <si>
-    <t>Clustered Index Size</t>
-  </si>
-  <si>
-    <t>Nonclustered Index Details</t>
-  </si>
-  <si>
-    <t>Size of the Nonclustered Index</t>
-  </si>
-  <si>
-    <t>Non-Leaf Index rows per page</t>
-  </si>
-  <si>
-    <t>Leaf Index Row Size</t>
-  </si>
-  <si>
-    <t>Leaf Index rows per page</t>
-  </si>
-  <si>
-    <t>NCI 90% Fill Factor</t>
-  </si>
-  <si>
-    <t>9.0</t>
-  </si>
-  <si>
-    <t>9.1</t>
-  </si>
-  <si>
-    <t>9.2</t>
-  </si>
-  <si>
-    <t>9.n</t>
-  </si>
-  <si>
-    <t>9.t</t>
-  </si>
-  <si>
-    <t>Database Size Per Node</t>
-  </si>
-  <si>
-    <t>Total Database Size (All Nodes)</t>
-  </si>
-  <si>
-    <t>Total Database Size</t>
-  </si>
-  <si>
-    <t>***Resources used for caluclations</t>
-  </si>
-  <si>
-    <t>Estimating the Size of a Table with a Clustered Index (SQL 2000)</t>
-  </si>
-  <si>
-    <t>http://msdn2.microsoft.com/en-us/library/aa933051(SQL.80).aspx</t>
-  </si>
-  <si>
-    <t>Estimating the Size of a Table (SQL 2000)</t>
-  </si>
-  <si>
-    <t>http://msdn2.microsoft.com/en-us/library/aa933068(SQL.80).aspx</t>
+    <t xml:space="preserve">Minimum Row size with varchar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average Row size with varchar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Row size with int</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">varchars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">varchar Max total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">null bitmap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">varchar estimated size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">varchar size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Row Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bytes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dci's</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nodes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">polling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seconds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">retention</t>
+  </si>
+  <si>
+    <t xml:space="preserve">days</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># of records per DCI</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># of records per node (# of rows)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># of records total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Size of SQL data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numer of rows per page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clustered Index - 90% fill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table Size (Data_Space_Used)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clustered Index Details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of Columns in Index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of Bytes of int cols in index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of varchar in index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max Size of varchar in index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">null bitmap in index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">varchar index size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Index Row Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Size of the Clustered Index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Index Rows Per page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pages Level 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pages Level 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pages Level 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{Note:  Repeat untl Pages Level n = 1}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Number of Pages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clustered Index Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nonclustered Index Details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Size of the Nonclustered Index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-Leaf Index rows per page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leaf Index Row Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leaf Index rows per page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NCI 90% Fill Factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database Size Per Node</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Database Size (All Nodes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Database Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">***Resources used for caluclations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimating the Size of a Table with a Clustered Index (SQL 2000)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://msdn2.microsoft.com/en-us/library/aa933051(SQL.80).aspx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimating the Size of a Table (SQL 2000)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://msdn2.microsoft.com/en-us/library/aa933068(SQL.80).aspx</t>
   </si>
 </sst>
 </file>
@@ -256,7 +261,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
@@ -708,25 +713,25 @@
   </sheetPr>
   <dimension ref="A1:P87"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A50" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J82" activeCellId="0" sqref="J82"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A47" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E82" activeCellId="0" sqref="E82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.14285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.1428571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.9948979591837"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.8520408163265"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.9948979591837"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="27.8520408163265"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.9948979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.72959183673469"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="8.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="8.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="8.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="27.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="8.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="8.72"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -846,7 +851,7 @@
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
       <c r="E4" s="12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="11" t="s">
@@ -879,7 +884,7 @@
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12" t="n">
-        <v>255</v>
+        <v>510</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="11" t="s">
@@ -946,7 +951,7 @@
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
       <c r="E7" s="12" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="11" t="s">
@@ -979,7 +984,7 @@
       <c r="D8" s="12"/>
       <c r="E8" s="12" t="n">
         <f aca="false">IF(E4=0,0,2+(E4*2)+E7)</f>
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="11" t="s">
@@ -1022,7 +1027,7 @@
       <c r="D9" s="12"/>
       <c r="E9" s="12" t="n">
         <f aca="false">E3+E8+E6+4</f>
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="F9" s="13" t="s">
         <v>18</v>
@@ -1091,7 +1096,7 @@
         <v>19</v>
       </c>
       <c r="C12" s="12" t="n">
-        <v>1769</v>
+        <v>12000</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
@@ -1120,7 +1125,7 @@
         <v>20</v>
       </c>
       <c r="C13" s="12" t="n">
-        <v>101</v>
+        <v>400</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
@@ -1184,7 +1189,7 @@
         <v>23</v>
       </c>
       <c r="C15" s="12" t="n">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>24</v>
@@ -1222,7 +1227,7 @@
       <c r="D16" s="12"/>
       <c r="E16" s="12" t="n">
         <f aca="false">C15*60*60*24/C14</f>
-        <v>43200</v>
+        <v>129600</v>
       </c>
       <c r="F16" s="13"/>
       <c r="G16" s="11" t="s">
@@ -1257,7 +1262,7 @@
       <c r="D17" s="12"/>
       <c r="E17" s="12" t="n">
         <f aca="false">ROUNDUP(E16*(C12/C13),0)</f>
-        <v>756642</v>
+        <v>3888000</v>
       </c>
       <c r="F17" s="13"/>
       <c r="G17" s="11" t="s">
@@ -1289,7 +1294,7 @@
       <c r="D18" s="12"/>
       <c r="E18" s="12" t="n">
         <f aca="false">E16*C12</f>
-        <v>76420800</v>
+        <v>1555200000</v>
       </c>
       <c r="F18" s="13"/>
       <c r="G18" s="11" t="s">
@@ -1382,7 +1387,7 @@
       <c r="D22" s="19"/>
       <c r="E22" s="19" t="n">
         <f aca="false">ROUNDDOWN((8096/(E9+2)),0)</f>
-        <v>337</v>
+        <v>269</v>
       </c>
       <c r="F22" s="20"/>
       <c r="G22" s="18" t="s">
@@ -1417,7 +1422,7 @@
       <c r="D23" s="19"/>
       <c r="E23" s="19" t="n">
         <f aca="false">ROUNDDOWN(8096*((100-90)/100)/(E9+2),0)</f>
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F23" s="20"/>
       <c r="G23" s="18" t="s">
@@ -1452,7 +1457,7 @@
       <c r="D24" s="19"/>
       <c r="E24" s="19" t="n">
         <f aca="false">ROUNDUP(E17/(E22-E23),0)</f>
-        <v>2489</v>
+        <v>16000</v>
       </c>
       <c r="F24" s="20"/>
       <c r="G24" s="18" t="s">
@@ -1487,7 +1492,7 @@
       <c r="D25" s="19"/>
       <c r="E25" s="19" t="n">
         <f aca="false">E24*8192</f>
-        <v>20389888</v>
+        <v>131072000</v>
       </c>
       <c r="F25" s="20" t="s">
         <v>18</v>
@@ -1523,7 +1528,7 @@
       <c r="D26" s="19"/>
       <c r="E26" s="19" t="n">
         <f aca="false">E25/1024</f>
-        <v>19912</v>
+        <v>128000</v>
       </c>
       <c r="F26" s="20" t="s">
         <v>33</v>
@@ -1555,7 +1560,7 @@
       <c r="D27" s="19"/>
       <c r="E27" s="21" t="n">
         <f aca="false">E26/1024</f>
-        <v>19.4453125</v>
+        <v>125</v>
       </c>
       <c r="F27" s="20" t="s">
         <v>34</v>
@@ -1587,7 +1592,7 @@
       <c r="D28" s="23"/>
       <c r="E28" s="24" t="n">
         <f aca="false">E27/1024</f>
-        <v>0.0189895629882813</v>
+        <v>0.1220703125</v>
       </c>
       <c r="F28" s="25" t="s">
         <v>35</v>
@@ -1977,7 +1982,7 @@
       <c r="D40" s="19"/>
       <c r="E40" s="19" t="n">
         <f aca="false">ROUNDUP(((E25/8192)/E39),0)</f>
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="F40" s="20"/>
       <c r="G40" s="18" t="s">
@@ -2108,7 +2113,7 @@
       <c r="D44" s="19"/>
       <c r="E44" s="19" t="n">
         <f aca="false">SUM(E40:E42)</f>
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="F44" s="20"/>
       <c r="G44" s="18" t="s">
@@ -2143,7 +2148,7 @@
       <c r="D45" s="19"/>
       <c r="E45" s="19" t="n">
         <f aca="false">8192*E44</f>
-        <v>65536</v>
+        <v>311296</v>
       </c>
       <c r="F45" s="20" t="s">
         <v>18</v>
@@ -2179,7 +2184,7 @@
       <c r="D46" s="19"/>
       <c r="E46" s="19" t="n">
         <f aca="false">E45/1024</f>
-        <v>64</v>
+        <v>304</v>
       </c>
       <c r="F46" s="20" t="s">
         <v>33</v>
@@ -2211,7 +2216,7 @@
       <c r="D47" s="19"/>
       <c r="E47" s="21" t="n">
         <f aca="false">E46/1024</f>
-        <v>0.0625</v>
+        <v>0.296875</v>
       </c>
       <c r="F47" s="20" t="s">
         <v>34</v>
@@ -2243,7 +2248,7 @@
       <c r="D48" s="23"/>
       <c r="E48" s="24" t="n">
         <f aca="false">E47/1024</f>
-        <v>6.103515625E-005</v>
+        <v>0.0002899169921875</v>
       </c>
       <c r="F48" s="25" t="s">
         <v>35</v>
@@ -2738,7 +2743,7 @@
       <c r="D63" s="19"/>
       <c r="E63" s="19" t="n">
         <f aca="false">ROUNDUP(E17/(E61-E62),0)</f>
-        <v>2514</v>
+        <v>12917</v>
       </c>
       <c r="F63" s="20"/>
       <c r="G63" s="18" t="s">
@@ -2773,7 +2778,7 @@
       <c r="D64" s="19"/>
       <c r="E64" s="19" t="n">
         <f aca="false">ROUNDUP(E63/E$59,0)</f>
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="F64" s="20"/>
       <c r="G64" s="18" t="s">
@@ -2869,7 +2874,7 @@
       <c r="D67" s="19"/>
       <c r="E67" s="19" t="n">
         <f aca="false">SUM(E63:E65)</f>
-        <v>2520</v>
+        <v>12944</v>
       </c>
       <c r="F67" s="20"/>
       <c r="G67" s="18" t="s">
@@ -2904,7 +2909,7 @@
       <c r="D68" s="19"/>
       <c r="E68" s="19" t="n">
         <f aca="false">8192*E67</f>
-        <v>20643840</v>
+        <v>106037248</v>
       </c>
       <c r="F68" s="20" t="s">
         <v>18</v>
@@ -2940,7 +2945,7 @@
       <c r="D69" s="19"/>
       <c r="E69" s="19" t="n">
         <f aca="false">E68/1024</f>
-        <v>20160</v>
+        <v>103552</v>
       </c>
       <c r="F69" s="20" t="s">
         <v>33</v>
@@ -2972,7 +2977,7 @@
       <c r="D70" s="19"/>
       <c r="E70" s="21" t="n">
         <f aca="false">E69/1024</f>
-        <v>19.6875</v>
+        <v>101.125</v>
       </c>
       <c r="F70" s="20" t="s">
         <v>34</v>
@@ -3004,7 +3009,7 @@
       <c r="D71" s="23"/>
       <c r="E71" s="24" t="n">
         <f aca="false">E70/1024</f>
-        <v>0.01922607421875</v>
+        <v>0.0987548828125</v>
       </c>
       <c r="F71" s="25" t="s">
         <v>35</v>
@@ -3037,7 +3042,7 @@
       </c>
       <c r="E73" s="31" t="n">
         <f aca="false">E68+E45+E25</f>
-        <v>41099264</v>
+        <v>237420544</v>
       </c>
       <c r="F73" s="31" t="s">
         <v>18</v>
@@ -3069,7 +3074,7 @@
       <c r="D74" s="31"/>
       <c r="E74" s="31" t="n">
         <f aca="false">E73/1024</f>
-        <v>40136</v>
+        <v>231856</v>
       </c>
       <c r="F74" s="31" t="s">
         <v>33</v>
@@ -3095,7 +3100,7 @@
       <c r="D75" s="31"/>
       <c r="E75" s="32" t="n">
         <f aca="false">E74/1024</f>
-        <v>39.1953125</v>
+        <v>226.421875</v>
       </c>
       <c r="F75" s="31" t="s">
         <v>34</v>
@@ -3121,7 +3126,7 @@
       <c r="D76" s="31"/>
       <c r="E76" s="33" t="n">
         <f aca="false">E75/1024</f>
-        <v>0.0382766723632812</v>
+        <v>0.221115112304687</v>
       </c>
       <c r="F76" s="31" t="s">
         <v>35</v>
@@ -3156,7 +3161,7 @@
       </c>
       <c r="E79" s="35" t="n">
         <f aca="false">E73*C13</f>
-        <v>4151025664</v>
+        <v>94968217600</v>
       </c>
       <c r="F79" s="35" t="s">
         <v>18</v>
@@ -3188,7 +3193,7 @@
       <c r="D80" s="35"/>
       <c r="E80" s="35" t="n">
         <f aca="false">E79/1024</f>
-        <v>4053736</v>
+        <v>92742400</v>
       </c>
       <c r="F80" s="35" t="s">
         <v>33</v>
@@ -3216,7 +3221,7 @@
       <c r="D81" s="35"/>
       <c r="E81" s="36" t="n">
         <f aca="false">E80/1024</f>
-        <v>3958.7265625</v>
+        <v>90568.75</v>
       </c>
       <c r="F81" s="35" t="s">
         <v>34</v>
@@ -3242,7 +3247,7 @@
       <c r="D82" s="35"/>
       <c r="E82" s="37" t="n">
         <f aca="false">E81/1024</f>
-        <v>3.86594390869141</v>
+        <v>88.446044921875</v>
       </c>
       <c r="F82" s="35" t="s">
         <v>35</v>
@@ -3332,7 +3337,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>